<commit_message>
Worked a little bit
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mary van Valkenburg\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\volun\Documents\DA13\Excel\lookups-exercise-volunteercjt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{19ED61FC-0AAB-4DAC-83F6-00D6AC42053B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD59FA1-C7AB-49EB-8F91-3C8AA71AA310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="135" yWindow="90" windowWidth="21877" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metro_budget" sheetId="1" r:id="rId1"/>
@@ -33,8 +33,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="90">
   <si>
     <t>Department</t>
   </si>
@@ -314,7 +336,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -454,11 +476,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -880,9 +904,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -920,7 +944,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1026,7 +1050,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1168,7 +1192,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1176,27 +1200,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P107"/>
+  <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="15.85546875" customWidth="1"/>
-    <col min="13" max="13" width="15.42578125" customWidth="1"/>
-    <col min="14" max="15" width="17.85546875" customWidth="1"/>
-    <col min="16" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" customWidth="1"/>
+    <col min="8" max="8" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="15.88671875" customWidth="1"/>
+    <col min="13" max="13" width="15.44140625" customWidth="1"/>
+    <col min="14" max="15" width="17.88671875" customWidth="1"/>
+    <col min="16" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1246,7 +1270,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1272,7 +1296,7 @@
       </c>
       <c r="O2" s="5"/>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1298,7 +1322,7 @@
       </c>
       <c r="O3" s="5"/>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1324,7 +1348,7 @@
       </c>
       <c r="O4" s="5"/>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1350,7 +1374,7 @@
       </c>
       <c r="O5" s="5"/>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1376,7 +1400,7 @@
       </c>
       <c r="O6" s="5"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1402,7 +1426,7 @@
       </c>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1428,7 +1452,7 @@
       </c>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1454,7 +1478,7 @@
       </c>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1480,7 +1504,7 @@
       </c>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1506,7 +1530,7 @@
       </c>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1532,7 +1556,7 @@
       </c>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1558,7 +1582,7 @@
       </c>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1584,7 +1608,7 @@
       </c>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1610,7 +1634,7 @@
       </c>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1636,7 +1660,7 @@
       </c>
       <c r="O16" s="5"/>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1662,7 +1686,7 @@
       </c>
       <c r="O17" s="5"/>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1688,7 +1712,7 @@
       </c>
       <c r="O18" s="5"/>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1714,7 +1738,7 @@
       </c>
       <c r="O19" s="5"/>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -1740,7 +1764,7 @@
       </c>
       <c r="O20" s="5"/>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -1766,7 +1790,7 @@
       </c>
       <c r="O21" s="5"/>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -1792,7 +1816,7 @@
       </c>
       <c r="O22" s="5"/>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -1818,7 +1842,7 @@
       </c>
       <c r="O23" s="5"/>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -1844,7 +1868,7 @@
       </c>
       <c r="O24" s="5"/>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -1870,7 +1894,7 @@
       </c>
       <c r="O25" s="5"/>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -1896,7 +1920,7 @@
       </c>
       <c r="O26" s="5"/>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -1922,7 +1946,7 @@
       </c>
       <c r="O27" s="5"/>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -1948,7 +1972,7 @@
       </c>
       <c r="O28" s="5"/>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -1974,7 +1998,7 @@
       </c>
       <c r="O29" s="5"/>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>44</v>
       </c>
@@ -2000,7 +2024,7 @@
       </c>
       <c r="O30" s="5"/>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>45</v>
       </c>
@@ -2026,7 +2050,7 @@
       </c>
       <c r="O31" s="5"/>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>46</v>
       </c>
@@ -2052,7 +2076,7 @@
       </c>
       <c r="O32" s="5"/>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>47</v>
       </c>
@@ -2078,7 +2102,7 @@
       </c>
       <c r="O33" s="5"/>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>48</v>
       </c>
@@ -2104,7 +2128,7 @@
       </c>
       <c r="O34" s="5"/>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>49</v>
       </c>
@@ -2130,7 +2154,7 @@
       </c>
       <c r="O35" s="5"/>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>50</v>
       </c>
@@ -2156,7 +2180,7 @@
       </c>
       <c r="O36" s="5"/>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>51</v>
       </c>
@@ -2182,7 +2206,7 @@
       </c>
       <c r="O37" s="5"/>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -2208,7 +2232,7 @@
       </c>
       <c r="O38" s="5"/>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>53</v>
       </c>
@@ -2234,7 +2258,7 @@
       </c>
       <c r="O39" s="5"/>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>54</v>
       </c>
@@ -2260,7 +2284,7 @@
       </c>
       <c r="O40" s="5"/>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>55</v>
       </c>
@@ -2286,7 +2310,7 @@
       </c>
       <c r="O41" s="5"/>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>56</v>
       </c>
@@ -2312,7 +2336,7 @@
       </c>
       <c r="O42" s="5"/>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>57</v>
       </c>
@@ -2338,7 +2362,7 @@
       </c>
       <c r="O43" s="5"/>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>58</v>
       </c>
@@ -2364,7 +2388,7 @@
       </c>
       <c r="O44" s="5"/>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>59</v>
       </c>
@@ -2390,7 +2414,7 @@
       </c>
       <c r="O45" s="5"/>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>60</v>
       </c>
@@ -2416,7 +2440,7 @@
       </c>
       <c r="O46" s="5"/>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>61</v>
       </c>
@@ -2442,7 +2466,7 @@
       </c>
       <c r="O47" s="5"/>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>62</v>
       </c>
@@ -2468,7 +2492,7 @@
       </c>
       <c r="O48" s="5"/>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>63</v>
       </c>
@@ -2494,7 +2518,7 @@
       </c>
       <c r="O49" s="5"/>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>64</v>
       </c>
@@ -2520,7 +2544,7 @@
       </c>
       <c r="O50" s="5"/>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>65</v>
       </c>
@@ -2546,7 +2570,7 @@
       </c>
       <c r="O51" s="5"/>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>66</v>
       </c>
@@ -2572,12 +2596,12 @@
       </c>
       <c r="O52" s="5"/>
     </row>
-    <row r="54" spans="1:15" ht="15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
@@ -2591,42 +2615,42 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="15">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="64" spans="1:15">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>0</v>
       </c>
@@ -2640,43 +2664,54 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" ht="15"/>
-    <row r="72" spans="1:4" ht="15">
+      <c r="H70" cm="1">
+        <f t="array" ref="H70:H73">INDEX(G49:G52,,1)</f>
+        <v>102600</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H71">
+        <v>859100</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" ht="15">
+      <c r="H72">
+        <v>8925500</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>0</v>
       </c>
@@ -2689,49 +2724,51 @@
       <c r="D73" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" ht="15">
+      <c r="H73">
+        <v>2440700</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15"/>
-    <row r="81" spans="1:7" ht="15">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="15">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B83" s="1" t="s">
         <v>71</v>
       </c>
@@ -2739,34 +2776,56 @@
         <v>72</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>73</v>
       </c>
-      <c r="B84" s="6"/>
-      <c r="C84" s="6"/>
-    </row>
-    <row r="85" spans="1:7">
+      <c r="B84" s="6">
+        <f>INDEX($A$2:$M$52,MATCH($B$87,$A$2:$A$52,0),MATCH(_xlfn.CONCAT($A84,"_",B$83),$A$1:$P$1,0))</f>
+        <v>2561800</v>
+      </c>
+      <c r="C84" s="6">
+        <f>INDEX($A$2:$M$52,MATCH($B$87,$A$2:$A$52,0),MATCH(_xlfn.CONCAT($A84,"_",C$83),$A$1:$P$1,0))</f>
+        <v>2523884.71</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>74</v>
       </c>
-      <c r="B85" s="6"/>
-      <c r="C85" s="6"/>
-    </row>
-    <row r="86" spans="1:7">
+      <c r="B85" s="6">
+        <f t="shared" ref="B85:C86" si="0">INDEX($A$2:$M$52,MATCH($B$87,$A$2:$A$52,0),MATCH(_xlfn.CONCAT($A85,"_",B$83),$A$1:$P$1,0))</f>
+        <v>2779500</v>
+      </c>
+      <c r="C85" s="6">
+        <f t="shared" si="0"/>
+        <v>2665264.4399999902</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>75</v>
       </c>
-      <c r="B86" s="6"/>
-      <c r="C86" s="6"/>
-    </row>
-    <row r="87" spans="1:7" ht="15"/>
-    <row r="88" spans="1:7" ht="15">
+      <c r="B86" s="6">
+        <f t="shared" si="0"/>
+        <v>2889900</v>
+      </c>
+      <c r="C86" s="6">
+        <f t="shared" si="0"/>
+        <v>2889864.67</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B87" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="15">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>77</v>
       </c>
@@ -2782,7 +2841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="15">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B90" s="8" t="s">
         <v>0</v>
       </c>
@@ -2802,7 +2861,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>73</v>
       </c>
@@ -2810,7 +2869,7 @@
       <c r="E91" s="5"/>
       <c r="G91" s="5"/>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>74</v>
       </c>
@@ -2818,7 +2877,7 @@
       <c r="E92" s="5"/>
       <c r="G92" s="5"/>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>75</v>
       </c>
@@ -2826,12 +2885,12 @@
       <c r="E93" s="5"/>
       <c r="G93" s="5"/>
     </row>
-    <row r="95" spans="1:7" ht="15">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="15">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>77</v>
       </c>
@@ -2847,7 +2906,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="15">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B97" s="8" t="s">
         <v>0</v>
       </c>
@@ -2867,7 +2926,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>73</v>
       </c>
@@ -2876,7 +2935,7 @@
       <c r="G98" s="4"/>
       <c r="I98" s="4"/>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>74</v>
       </c>
@@ -2885,7 +2944,7 @@
       <c r="G99" s="4"/>
       <c r="I99" s="4"/>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>75</v>
       </c>
@@ -2894,15 +2953,9 @@
       <c r="G100" s="4"/>
       <c r="I100" s="4"/>
     </row>
-    <row r="102" spans="1:9" ht="15"/>
-    <row r="103" spans="1:9" ht="15"/>
-    <row r="104" spans="1:9" ht="15"/>
-    <row r="105" spans="1:9" ht="15"/>
-    <row r="106" spans="1:9" ht="15"/>
-    <row r="107" spans="1:9" ht="15"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83 B87" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
       <formula1>$A$2:$A$52</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82:B83" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>
@@ -2919,13 +2972,13 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2933,7 +2986,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2941,7 +2994,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2949,7 +3002,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -2957,7 +3010,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -2965,7 +3018,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -2973,7 +3026,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -2981,7 +3034,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -2989,7 +3042,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -2997,7 +3050,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>

</xml_diff>